<commit_message>
typo fix, notation clarification on negative sampling
</commit_message>
<xml_diff>
--- a/downloads/notebooks/word2vec_numerical_demo.xlsx
+++ b/downloads/notebooks/word2vec_numerical_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricKim\Documents\aegis4048.github.io-source\content\downloads\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9B9827-B0C4-4FD3-912B-20945DAAF24F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E570EBD7-54BF-4C5B-8B36-B26CFD92107E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="7" xr2:uid="{1F5C5C51-52F8-4C6D-9E63-A97493B2A8A4}"/>
+    <workbookView minimized="1" xWindow="3876" yWindow="366" windowWidth="11310" windowHeight="12594" activeTab="1" xr2:uid="{1F5C5C51-52F8-4C6D-9E63-A97493B2A8A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="neg_demo" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="A">Sheet1!$D$7:$D$14</definedName>
@@ -940,30 +941,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1000,6 +977,57 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,33 +1055,6 @@
     <xf numFmtId="164" fontId="9" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10180,8 +10181,8 @@
       <xdr:rowOff>213360</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -10245,7 +10246,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -10311,8 +10312,8 @@
       <xdr:rowOff>220980</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="241156" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -10376,7 +10377,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -10508,8 +10509,8 @@
       <xdr:rowOff>229887</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -10573,7 +10574,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -12245,8 +12246,8 @@
       <xdr:rowOff>213360</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="43" name="TextBox 42">
@@ -12310,7 +12311,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="43" name="TextBox 42">
@@ -12376,8 +12377,8 @@
       <xdr:rowOff>220980</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="241156" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="44" name="TextBox 43">
@@ -12441,7 +12442,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="44" name="TextBox 43">
@@ -12573,8 +12574,8 @@
       <xdr:rowOff>229887</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="47" name="TextBox 46">
@@ -12638,7 +12639,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="47" name="TextBox 46">
@@ -14189,8 +14190,8 @@
       <xdr:rowOff>213360</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="80" name="TextBox 79">
@@ -14254,7 +14255,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="80" name="TextBox 79">
@@ -14320,8 +14321,8 @@
       <xdr:rowOff>220980</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="241156" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="81" name="TextBox 80">
@@ -14385,7 +14386,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="81" name="TextBox 80">
@@ -14517,8 +14518,8 @@
       <xdr:rowOff>229887</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="84" name="TextBox 83">
@@ -14582,7 +14583,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="84" name="TextBox 83">
@@ -16298,8 +16299,8 @@
       <xdr:rowOff>213360</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="117" name="TextBox 116">
@@ -16363,7 +16364,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="117" name="TextBox 116">
@@ -16429,8 +16430,8 @@
       <xdr:rowOff>220980</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="241156" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="118" name="TextBox 117">
@@ -16494,7 +16495,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="118" name="TextBox 117">
@@ -16626,8 +16627,8 @@
       <xdr:rowOff>229887</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="249555" cy="313099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="121" name="TextBox 120">
@@ -16691,7 +16692,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="121" name="TextBox 120">
@@ -58158,8 +58159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B5FEC7-FC6A-4142-907B-9AC559732443}">
   <dimension ref="B2:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -58172,30 +58173,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="45.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
     </row>
     <row r="4" spans="2:10" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
+      <c r="C4" s="138"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
     </row>
     <row r="5" spans="2:10" ht="7.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="2"/>
@@ -58238,7 +58239,7 @@
       <c r="D7" s="9">
         <v>0</v>
       </c>
-      <c r="E7" s="98"/>
+      <c r="E7" s="137"/>
       <c r="F7" s="14">
         <v>-7.8E-2</v>
       </c>
@@ -58248,7 +58249,7 @@
       <c r="H7" s="16">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="I7" s="98"/>
+      <c r="I7" s="137"/>
       <c r="J7" s="30">
         <f t="array" ref="J7:J9">TRANSPOSE(MMULT(TRANSPOSE(A), B))</f>
         <v>6.8000000000000005E-2</v>
@@ -58264,7 +58265,7 @@
       <c r="D8" s="44">
         <v>1</v>
       </c>
-      <c r="E8" s="98"/>
+      <c r="E8" s="137"/>
       <c r="F8" s="81">
         <v>6.8000000000000005E-2</v>
       </c>
@@ -58274,7 +58275,7 @@
       <c r="H8" s="83">
         <v>-0.109</v>
       </c>
-      <c r="I8" s="98"/>
+      <c r="I8" s="137"/>
       <c r="J8" s="31">
         <v>0.17</v>
       </c>
@@ -58289,7 +58290,7 @@
       <c r="D9" s="10">
         <v>0</v>
       </c>
-      <c r="E9" s="98"/>
+      <c r="E9" s="137"/>
       <c r="F9" s="17">
         <v>-0.158</v>
       </c>
@@ -58299,7 +58300,7 @@
       <c r="H9" s="19">
         <v>-0.151</v>
       </c>
-      <c r="I9" s="98"/>
+      <c r="I9" s="137"/>
       <c r="J9" s="32">
         <v>-0.109</v>
       </c>
@@ -58314,7 +58315,7 @@
       <c r="D10" s="10">
         <v>0</v>
       </c>
-      <c r="E10" s="98"/>
+      <c r="E10" s="137"/>
       <c r="F10" s="17">
         <v>0.15</v>
       </c>
@@ -58324,7 +58325,7 @@
       <c r="H10" s="19">
         <v>0.14499999999999999</v>
       </c>
-      <c r="I10" s="98"/>
+      <c r="I10" s="137"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -58337,7 +58338,7 @@
       <c r="D11" s="10">
         <v>0</v>
       </c>
-      <c r="E11" s="98"/>
+      <c r="E11" s="137"/>
       <c r="F11" s="17">
         <v>-9.7000000000000003E-2</v>
       </c>
@@ -58347,7 +58348,7 @@
       <c r="H11" s="19">
         <v>0.188</v>
       </c>
-      <c r="I11" s="98"/>
+      <c r="I11" s="137"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -58360,7 +58361,7 @@
       <c r="D12" s="10">
         <v>0</v>
       </c>
-      <c r="E12" s="98"/>
+      <c r="E12" s="137"/>
       <c r="F12" s="17">
         <v>3.5999999999999997E-2</v>
       </c>
@@ -58370,7 +58371,7 @@
       <c r="H12" s="19">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="I12" s="98"/>
+      <c r="I12" s="137"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -58383,7 +58384,7 @@
       <c r="D13" s="42">
         <v>0</v>
       </c>
-      <c r="E13" s="98"/>
+      <c r="E13" s="137"/>
       <c r="F13" s="17">
         <v>0.16800000000000001</v>
       </c>
@@ -58393,7 +58394,7 @@
       <c r="H13" s="19">
         <v>-5.8000000000000003E-2</v>
       </c>
-      <c r="I13" s="98"/>
+      <c r="I13" s="137"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -58406,7 +58407,7 @@
       <c r="D14" s="43">
         <v>0</v>
       </c>
-      <c r="E14" s="98"/>
+      <c r="E14" s="137"/>
       <c r="F14" s="20">
         <v>9.8000000000000004E-2</v>
       </c>
@@ -58416,7 +58417,7 @@
       <c r="H14" s="22">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="I14" s="98"/>
+      <c r="I14" s="137"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="2:10" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
@@ -58456,7 +58457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9E3C9C-B15E-4422-9BFC-70661AC95FB9}">
   <dimension ref="B2:S34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -58470,18 +58471,18 @@
   <sheetData>
     <row r="2" spans="2:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="49"/>
-      <c r="C2" s="99" t="s">
+      <c r="C2" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
     </row>
     <row r="3" spans="2:19" ht="7.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="2"/>
@@ -58551,10 +58552,10 @@
       <c r="I6" s="34">
         <v>2.0144000000000002E-2</v>
       </c>
-      <c r="J6" s="100" t="s">
+      <c r="J6" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="101"/>
+      <c r="K6" s="140"/>
       <c r="L6" s="24">
         <f t="shared" si="0"/>
         <v>0.20122717463313133</v>
@@ -58577,10 +58578,10 @@
       <c r="I7" s="34">
         <v>6.3549999999999995E-3</v>
       </c>
-      <c r="J7" s="102" t="s">
+      <c r="J7" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="103"/>
+      <c r="K7" s="142"/>
       <c r="L7" s="24">
         <f t="shared" si="0"/>
         <v>0.19847149581253729</v>
@@ -58695,10 +58696,10 @@
       <c r="I13" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="103" t="s">
+      <c r="J13" s="142" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="103"/>
+      <c r="K13" s="142"/>
       <c r="L13" s="12">
         <v>1</v>
       </c>
@@ -58712,8 +58713,8 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
+      <c r="J14" s="143"/>
+      <c r="K14" s="143"/>
       <c r="L14" s="13" t="s">
         <v>23</v>
       </c>
@@ -58802,21 +58803,21 @@
   <sheetData>
     <row r="2" spans="2:19" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="49"/>
-      <c r="C2" s="99" t="s">
+      <c r="C2" s="138" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
+      <c r="O2" s="138"/>
     </row>
     <row r="3" spans="2:19" ht="7.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="2"/>
@@ -59208,16 +59209,16 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="2" spans="2:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="138" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
       <c r="J2" s="49"/>
     </row>
     <row r="3" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -59255,7 +59256,7 @@
         <f>Sheet2!G5</f>
         <v>1.2E-2</v>
       </c>
-      <c r="E5" s="98"/>
+      <c r="E5" s="137"/>
       <c r="F5" s="52">
         <f>Sheet3!O5</f>
         <v>0.41121067419698687</v>
@@ -59278,7 +59279,7 @@
         <f>Sheet2!G6</f>
         <v>-4.5999999999999999E-2</v>
       </c>
-      <c r="E6" s="98"/>
+      <c r="E6" s="137"/>
       <c r="F6" s="53">
         <f>Sheet3!O6</f>
         <v>0.40245434926626267</v>
@@ -59300,7 +59301,7 @@
         <f>Sheet2!G7</f>
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="E7" s="98"/>
+      <c r="E7" s="137"/>
       <c r="F7" s="53">
         <f>Sheet3!O7</f>
         <v>0.82242134839397374</v>
@@ -59322,7 +59323,7 @@
         <f>Sheet2!G8</f>
         <v>-4.3999999999999997E-2</v>
       </c>
-      <c r="E8" s="98"/>
+      <c r="E8" s="137"/>
       <c r="F8" s="53">
         <f>Sheet3!O8</f>
         <v>0.39710696293836123</v>
@@ -59345,7 +59346,7 @@
         <f>Sheet2!G9</f>
         <v>0.14699999999999999</v>
       </c>
-      <c r="E9" s="98"/>
+      <c r="E9" s="137"/>
       <c r="F9" s="53">
         <f>Sheet3!O9</f>
         <v>0.39228502197331472</v>
@@ -59368,7 +59369,7 @@
         <f>Sheet2!G10</f>
         <v>-9.7000000000000003E-2</v>
       </c>
-      <c r="E10" s="98"/>
+      <c r="E10" s="137"/>
       <c r="F10" s="53">
         <f>Sheet3!O10</f>
         <v>0.40657347885931561</v>
@@ -59391,7 +59392,7 @@
         <f>Sheet2!G11</f>
         <v>-0.19800000000000001</v>
       </c>
-      <c r="E11" s="98"/>
+      <c r="E11" s="137"/>
       <c r="F11" s="54">
         <f>Sheet3!O11</f>
         <v>-0.58434413410746155</v>
@@ -59414,7 +59415,7 @@
         <f>Sheet2!G12</f>
         <v>0.14799999999999999</v>
       </c>
-      <c r="E12" s="98"/>
+      <c r="E12" s="137"/>
       <c r="F12" s="55">
         <f>Sheet3!O12</f>
         <v>-0.6136739614277642</v>
@@ -59466,7 +59467,7 @@
       <c r="D18" s="9">
         <v>0</v>
       </c>
-      <c r="E18" s="98"/>
+      <c r="E18" s="137"/>
       <c r="F18" s="56">
         <f>H5</f>
         <v>6.6815342117344009E-2</v>
@@ -59492,7 +59493,7 @@
       <c r="D19" s="44">
         <v>1</v>
       </c>
-      <c r="E19" s="98"/>
+      <c r="E19" s="137"/>
       <c r="F19" s="57">
         <f t="shared" ref="F19:F20" si="0">H6</f>
         <v>0.17450004604327138</v>
@@ -59517,7 +59518,7 @@
       <c r="D20" s="10">
         <v>0</v>
       </c>
-      <c r="E20" s="98"/>
+      <c r="E20" s="137"/>
       <c r="F20" s="58">
         <f t="shared" si="0"/>
         <v>8.0314556614219629E-2</v>
@@ -59542,7 +59543,7 @@
       <c r="D21" s="10">
         <v>0</v>
       </c>
-      <c r="E21" s="98"/>
+      <c r="E21" s="137"/>
       <c r="F21" s="1"/>
       <c r="H21" s="59">
         <v>0</v>
@@ -59564,7 +59565,7 @@
       <c r="D22" s="10">
         <v>0</v>
       </c>
-      <c r="E22" s="98"/>
+      <c r="E22" s="137"/>
       <c r="F22" s="1"/>
       <c r="H22" s="59">
         <v>0</v>
@@ -59586,7 +59587,7 @@
       <c r="D23" s="10">
         <v>0</v>
       </c>
-      <c r="E23" s="98"/>
+      <c r="E23" s="137"/>
       <c r="F23" s="1"/>
       <c r="H23" s="59">
         <v>0</v>
@@ -59608,7 +59609,7 @@
       <c r="D24" s="42">
         <v>0</v>
       </c>
-      <c r="E24" s="98"/>
+      <c r="E24" s="137"/>
       <c r="F24" s="1"/>
       <c r="H24" s="59">
         <v>0</v>
@@ -59634,7 +59635,7 @@
       <c r="D25" s="43">
         <v>0</v>
       </c>
-      <c r="E25" s="98"/>
+      <c r="E25" s="137"/>
       <c r="F25" s="1"/>
       <c r="H25" s="59">
         <v>0</v>
@@ -59692,17 +59693,17 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="2" spans="2:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="138" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
       <c r="K2" s="49"/>
       <c r="L2" s="49"/>
       <c r="M2" s="49"/>
@@ -59900,21 +59901,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="138" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
       <c r="O2" s="49"/>
     </row>
     <row r="3" spans="2:15" ht="7.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -60273,7 +60274,7 @@
   <dimension ref="B2:O13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -60284,21 +60285,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="138" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
       <c r="O2" s="49"/>
     </row>
     <row r="3" spans="2:15" ht="7.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -60656,8 +60657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F629630E-960C-4802-A00C-FAAB9CE2CA8B}">
   <dimension ref="A2:R30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -60668,19 +60669,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
       <c r="O2" s="49"/>
     </row>
     <row r="3" spans="2:15" ht="7.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -60720,24 +60721,24 @@
       <c r="F5" s="1">
         <v>0.05</v>
       </c>
-      <c r="H5" s="105">
+      <c r="H5" s="97">
         <v>6.4199999999999993E-2</v>
       </c>
-      <c r="I5" s="106">
+      <c r="I5" s="98">
         <v>7.0900000000000005E-2</v>
       </c>
-      <c r="J5" s="107">
+      <c r="J5" s="99">
         <v>-1.41E-2</v>
       </c>
-      <c r="L5" s="119">
+      <c r="L5" s="111">
         <f>B5-$F$5*H5</f>
         <v>-0.5632100000000001</v>
       </c>
-      <c r="M5" s="120">
+      <c r="M5" s="112">
         <f t="shared" ref="M5:N5" si="0">C5-$F$5*I5</f>
         <v>0.336455</v>
       </c>
-      <c r="N5" s="121">
+      <c r="N5" s="113">
         <f t="shared" si="0"/>
         <v>0.16070500000000001</v>
       </c>
@@ -60752,24 +60753,24 @@
       <c r="D6" s="93">
         <v>1.56</v>
       </c>
-      <c r="H6" s="108">
+      <c r="H6" s="100">
         <v>9.8400000000000001E-2</v>
       </c>
       <c r="I6" s="64">
         <v>1.46E-2</v>
       </c>
-      <c r="J6" s="109">
+      <c r="J6" s="101">
         <v>6.2600000000000003E-2</v>
       </c>
-      <c r="L6" s="113">
+      <c r="L6" s="105">
         <f t="shared" ref="L6:L15" si="1">B6-$F$5*H6</f>
         <v>-0.91492000000000007</v>
       </c>
-      <c r="M6" s="114">
+      <c r="M6" s="106">
         <f t="shared" ref="M6:M15" si="2">C6-$F$5*I6</f>
         <v>-0.44073000000000001</v>
       </c>
-      <c r="N6" s="115">
+      <c r="N6" s="107">
         <f t="shared" ref="N6:N15" si="3">D6-$F$5*J6</f>
         <v>1.55687</v>
       </c>
@@ -60784,24 +60785,24 @@
       <c r="D7" s="93">
         <v>-1.32</v>
       </c>
-      <c r="H7" s="108">
+      <c r="H7" s="100">
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="I7" s="64">
         <v>8.9399999999999993E-2</v>
       </c>
-      <c r="J7" s="109">
+      <c r="J7" s="101">
         <v>4.4499999999999998E-2</v>
       </c>
-      <c r="L7" s="113">
+      <c r="L7" s="105">
         <f t="shared" si="1"/>
         <v>-1.2134499999999999</v>
       </c>
-      <c r="M7" s="114">
+      <c r="M7" s="106">
         <f t="shared" si="2"/>
         <v>-0.13447000000000001</v>
       </c>
-      <c r="N7" s="115">
+      <c r="N7" s="107">
         <f t="shared" si="3"/>
         <v>-1.322225</v>
       </c>
@@ -60816,24 +60817,24 @@
       <c r="D8" s="93">
         <v>-1.03</v>
       </c>
-      <c r="H8" s="108">
+      <c r="H8" s="100">
         <v>1.41E-2</v>
       </c>
       <c r="I8" s="64">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="J8" s="109">
+      <c r="J8" s="101">
         <v>7.8799999999999995E-2</v>
       </c>
-      <c r="L8" s="113">
+      <c r="L8" s="105">
         <f t="shared" si="1"/>
         <v>1.669295</v>
       </c>
-      <c r="M8" s="114">
+      <c r="M8" s="106">
         <f t="shared" si="2"/>
         <v>-0.15425</v>
       </c>
-      <c r="N8" s="115">
+      <c r="N8" s="107">
         <f t="shared" si="3"/>
         <v>-1.0339400000000001</v>
       </c>
@@ -60848,24 +60849,24 @@
       <c r="D9" s="93">
         <v>0.73</v>
       </c>
-      <c r="H9" s="108">
+      <c r="H9" s="100">
         <v>-2.0500000000000001E-2</v>
       </c>
       <c r="I9" s="64">
         <v>6.7400000000000002E-2</v>
       </c>
-      <c r="J9" s="109">
+      <c r="J9" s="101">
         <v>7.0599999999999996E-2</v>
       </c>
-      <c r="L9" s="113">
+      <c r="L9" s="105">
         <f t="shared" si="1"/>
         <v>1.721025</v>
       </c>
-      <c r="M9" s="114">
+      <c r="M9" s="106">
         <f t="shared" si="2"/>
         <v>-1.4633700000000001</v>
       </c>
-      <c r="N9" s="115">
+      <c r="N9" s="107">
         <f t="shared" si="3"/>
         <v>0.72646999999999995</v>
       </c>
@@ -60880,24 +60881,24 @@
       <c r="D10" s="93">
         <v>-0.12</v>
       </c>
-      <c r="H10" s="108">
+      <c r="H10" s="100">
         <v>-9.7900000000000001E-2</v>
       </c>
       <c r="I10" s="64">
         <v>-8.77E-2</v>
       </c>
-      <c r="J10" s="109">
+      <c r="J10" s="101">
         <v>9.1399999999999995E-2</v>
       </c>
-      <c r="L10" s="113">
+      <c r="L10" s="105">
         <f t="shared" si="1"/>
         <v>4.895E-3</v>
       </c>
-      <c r="M10" s="114">
+      <c r="M10" s="106">
         <f t="shared" si="2"/>
         <v>1.394385</v>
       </c>
-      <c r="N10" s="115">
+      <c r="N10" s="107">
         <f t="shared" si="3"/>
         <v>-0.12457</v>
       </c>
@@ -60912,24 +60913,24 @@
       <c r="D11" s="93">
         <v>-0.79</v>
       </c>
-      <c r="H11" s="108">
+      <c r="H11" s="100">
         <v>-7.17E-2</v>
       </c>
       <c r="I11" s="64">
         <v>-7.7499999999999999E-2</v>
       </c>
-      <c r="J11" s="109">
+      <c r="J11" s="101">
         <v>-8.9099999999999999E-2</v>
       </c>
-      <c r="L11" s="113">
+      <c r="L11" s="105">
         <f t="shared" si="1"/>
         <v>-5.6415E-2</v>
       </c>
-      <c r="M11" s="114">
+      <c r="M11" s="106">
         <f t="shared" si="2"/>
         <v>1.5238750000000001</v>
       </c>
-      <c r="N11" s="115">
+      <c r="N11" s="107">
         <f t="shared" si="3"/>
         <v>-0.78554500000000005</v>
       </c>
@@ -60944,24 +60945,24 @@
       <c r="D12" s="93">
         <v>-1.67</v>
       </c>
-      <c r="H12" s="108">
+      <c r="H12" s="100">
         <v>4.58E-2</v>
       </c>
       <c r="I12" s="64">
         <v>-7.8899999999999998E-2</v>
       </c>
-      <c r="J12" s="109">
+      <c r="J12" s="101">
         <v>-5.3199999999999997E-2</v>
       </c>
-      <c r="L12" s="113">
+      <c r="L12" s="105">
         <f t="shared" si="1"/>
         <v>0.79771000000000003</v>
       </c>
-      <c r="M12" s="114">
+      <c r="M12" s="106">
         <f t="shared" si="2"/>
         <v>1.8539450000000002</v>
       </c>
-      <c r="N12" s="115">
+      <c r="N12" s="107">
         <f t="shared" si="3"/>
         <v>-1.6673399999999998</v>
       </c>
@@ -60976,24 +60977,24 @@
       <c r="D13" s="93">
         <v>-0.48</v>
       </c>
-      <c r="H13" s="108">
+      <c r="H13" s="100">
         <v>-4.9399999999999999E-2</v>
       </c>
       <c r="I13" s="64">
         <v>-8.6900000000000005E-2</v>
       </c>
-      <c r="J13" s="109">
+      <c r="J13" s="101">
         <v>2.47E-2</v>
       </c>
-      <c r="L13" s="113">
+      <c r="L13" s="105">
         <f t="shared" si="1"/>
         <v>-1.3675300000000001</v>
       </c>
-      <c r="M13" s="114">
+      <c r="M13" s="106">
         <f t="shared" si="2"/>
         <v>1.3243450000000001</v>
       </c>
-      <c r="N13" s="115">
+      <c r="N13" s="107">
         <f t="shared" si="3"/>
         <v>-0.48123499999999997</v>
       </c>
@@ -61008,24 +61009,24 @@
       <c r="D14" s="93">
         <v>-1.85</v>
       </c>
-      <c r="H14" s="108">
+      <c r="H14" s="100">
         <v>-5.96E-2</v>
       </c>
       <c r="I14" s="64">
         <v>9.2299999999999993E-2</v>
       </c>
-      <c r="J14" s="109">
+      <c r="J14" s="101">
         <v>4.1799999999999997E-2</v>
       </c>
-      <c r="L14" s="113">
+      <c r="L14" s="105">
         <f t="shared" si="1"/>
         <v>0.67298000000000002</v>
       </c>
-      <c r="M14" s="114">
+      <c r="M14" s="106">
         <f t="shared" si="2"/>
         <v>1.985385</v>
       </c>
-      <c r="N14" s="115">
+      <c r="N14" s="107">
         <f t="shared" si="3"/>
         <v>-1.85209</v>
       </c>
@@ -61040,24 +61041,24 @@
       <c r="D15" s="96">
         <v>-1.86</v>
       </c>
-      <c r="H15" s="110">
+      <c r="H15" s="102">
         <v>7.3899999999999993E-2</v>
       </c>
-      <c r="I15" s="111">
+      <c r="I15" s="103">
         <v>5.0200000000000002E-2</v>
       </c>
-      <c r="J15" s="112">
+      <c r="J15" s="104">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L15" s="116">
+      <c r="L15" s="108">
         <f t="shared" si="1"/>
         <v>-1.523695</v>
       </c>
-      <c r="M15" s="117">
+      <c r="M15" s="109">
         <f t="shared" si="2"/>
         <v>-1.74251</v>
       </c>
-      <c r="N15" s="118">
+      <c r="N15" s="110">
         <f t="shared" si="3"/>
         <v>-1.8635000000000002</v>
       </c>
@@ -61111,23 +61112,23 @@
       <c r="F19" s="1">
         <v>0.05</v>
       </c>
-      <c r="H19" s="129" t="s">
+      <c r="H19" s="148" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="130"/>
-      <c r="J19" s="131"/>
-      <c r="L19" s="122">
+      <c r="I19" s="149"/>
+      <c r="J19" s="150"/>
+      <c r="L19" s="114">
         <v>-0.56000000000000005</v>
       </c>
-      <c r="M19" s="123">
+      <c r="M19" s="115">
         <v>0.34</v>
       </c>
-      <c r="N19" s="124">
+      <c r="N19" s="116">
         <v>0.16</v>
       </c>
-      <c r="P19" s="154"/>
-      <c r="Q19" s="155"/>
-      <c r="R19" s="156"/>
+      <c r="P19" s="133"/>
+      <c r="Q19" s="134"/>
+      <c r="R19" s="135"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="92">
@@ -61139,16 +61140,16 @@
       <c r="D20" s="93">
         <v>1.56</v>
       </c>
-      <c r="H20" s="132"/>
-      <c r="I20" s="133"/>
-      <c r="J20" s="134"/>
-      <c r="L20" s="125">
+      <c r="H20" s="151"/>
+      <c r="I20" s="152"/>
+      <c r="J20" s="153"/>
+      <c r="L20" s="117">
         <v>-0.91</v>
       </c>
-      <c r="M20" s="126">
+      <c r="M20" s="118">
         <v>-0.44</v>
       </c>
-      <c r="N20" s="127">
+      <c r="N20" s="119">
         <v>1.56</v>
       </c>
     </row>
@@ -61162,16 +61163,16 @@
       <c r="D21" s="93">
         <v>-1.32</v>
       </c>
-      <c r="H21" s="132"/>
-      <c r="I21" s="133"/>
-      <c r="J21" s="134"/>
-      <c r="L21" s="125">
+      <c r="H21" s="151"/>
+      <c r="I21" s="152"/>
+      <c r="J21" s="153"/>
+      <c r="L21" s="117">
         <v>-1.21</v>
       </c>
-      <c r="M21" s="126">
+      <c r="M21" s="118">
         <v>-0.13</v>
       </c>
-      <c r="N21" s="127">
+      <c r="N21" s="119">
         <v>-1.32</v>
       </c>
     </row>
@@ -61185,16 +61186,16 @@
       <c r="D22" s="93">
         <v>-1.03</v>
       </c>
-      <c r="H22" s="132"/>
-      <c r="I22" s="133"/>
-      <c r="J22" s="134"/>
-      <c r="L22" s="125">
+      <c r="H22" s="151"/>
+      <c r="I22" s="152"/>
+      <c r="J22" s="153"/>
+      <c r="L22" s="117">
         <v>1.67</v>
       </c>
-      <c r="M22" s="126">
+      <c r="M22" s="118">
         <v>-0.15</v>
       </c>
-      <c r="N22" s="127">
+      <c r="N22" s="119">
         <v>-1.03</v>
       </c>
     </row>
@@ -61208,16 +61209,16 @@
       <c r="D23" s="93">
         <v>0.73</v>
       </c>
-      <c r="H23" s="132"/>
-      <c r="I23" s="133"/>
-      <c r="J23" s="134"/>
-      <c r="L23" s="125">
+      <c r="H23" s="151"/>
+      <c r="I23" s="152"/>
+      <c r="J23" s="153"/>
+      <c r="L23" s="117">
         <v>1.72</v>
       </c>
-      <c r="M23" s="126">
+      <c r="M23" s="118">
         <v>-1.46</v>
       </c>
-      <c r="N23" s="127">
+      <c r="N23" s="119">
         <v>0.73</v>
       </c>
     </row>
@@ -61231,16 +61232,16 @@
       <c r="D24" s="93">
         <v>-0.12</v>
       </c>
-      <c r="H24" s="135"/>
-      <c r="I24" s="136"/>
-      <c r="J24" s="137"/>
-      <c r="L24" s="125">
+      <c r="H24" s="154"/>
+      <c r="I24" s="155"/>
+      <c r="J24" s="156"/>
+      <c r="L24" s="117">
         <v>0</v>
       </c>
-      <c r="M24" s="126">
+      <c r="M24" s="118">
         <v>1.39</v>
       </c>
-      <c r="N24" s="127">
+      <c r="N24" s="119">
         <v>-0.12</v>
       </c>
     </row>
@@ -61254,16 +61255,16 @@
       <c r="D25" s="93">
         <v>-0.79</v>
       </c>
-      <c r="H25" s="128"/>
-      <c r="I25" s="128"/>
-      <c r="J25" s="128"/>
-      <c r="L25" s="125">
+      <c r="H25" s="120"/>
+      <c r="I25" s="120"/>
+      <c r="J25" s="120"/>
+      <c r="L25" s="117">
         <v>-0.06</v>
       </c>
-      <c r="M25" s="126">
+      <c r="M25" s="118">
         <v>1.52</v>
       </c>
-      <c r="N25" s="127">
+      <c r="N25" s="119">
         <v>-0.79</v>
       </c>
     </row>
@@ -61277,29 +61278,29 @@
       <c r="D26" s="93">
         <v>-1.67</v>
       </c>
-      <c r="E26" s="151" t="s">
+      <c r="E26" s="144" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="152"/>
-      <c r="G26" s="153"/>
-      <c r="H26" s="148">
+      <c r="F26" s="145"/>
+      <c r="G26" s="146"/>
+      <c r="H26" s="130">
         <v>3.0499999999999999E-2</v>
       </c>
-      <c r="I26" s="149">
+      <c r="I26" s="131">
         <v>0.03</v>
       </c>
-      <c r="J26" s="150">
+      <c r="J26" s="132">
         <v>4.1200000000000001E-2</v>
       </c>
-      <c r="L26" s="145">
+      <c r="L26" s="127">
         <f>B26-0.05*H26</f>
         <v>0.79847500000000005</v>
       </c>
-      <c r="M26" s="146">
+      <c r="M26" s="128">
         <f t="shared" ref="M26:N26" si="4">C26-0.05*I26</f>
         <v>1.8485</v>
       </c>
-      <c r="N26" s="147">
+      <c r="N26" s="129">
         <f t="shared" si="4"/>
         <v>-1.6720599999999999</v>
       </c>
@@ -61314,29 +61315,29 @@
       <c r="D27" s="93">
         <v>-0.48</v>
       </c>
-      <c r="E27" s="151" t="s">
+      <c r="E27" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="152"/>
-      <c r="G27" s="153"/>
-      <c r="H27" s="108">
+      <c r="F27" s="145"/>
+      <c r="G27" s="146"/>
+      <c r="H27" s="100">
         <v>-8.9599999999999999E-2</v>
       </c>
       <c r="I27" s="64">
         <v>3.09E-2</v>
       </c>
-      <c r="J27" s="109">
+      <c r="J27" s="101">
         <v>-6.4500000000000002E-2</v>
       </c>
-      <c r="L27" s="138">
+      <c r="L27" s="121">
         <f t="shared" ref="L27:L29" si="5">B27-0.05*H27</f>
         <v>-1.3655200000000001</v>
       </c>
-      <c r="M27" s="139">
+      <c r="M27" s="122">
         <f t="shared" ref="M27:M29" si="6">C27-0.05*I27</f>
         <v>1.3184550000000002</v>
       </c>
-      <c r="N27" s="140">
+      <c r="N27" s="123">
         <f t="shared" ref="N27:N29" si="7">D27-0.05*J27</f>
         <v>-0.476775</v>
       </c>
@@ -61351,29 +61352,29 @@
       <c r="D28" s="93">
         <v>-1.85</v>
       </c>
-      <c r="E28" s="151" t="s">
+      <c r="E28" s="144" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="152"/>
-      <c r="G28" s="153"/>
-      <c r="H28" s="108">
+      <c r="F28" s="145"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="100">
         <v>5.5899999999999998E-2</v>
       </c>
       <c r="I28" s="64">
         <v>9.7900000000000001E-2</v>
       </c>
-      <c r="J28" s="109">
+      <c r="J28" s="101">
         <v>-6.08E-2</v>
       </c>
-      <c r="L28" s="138">
+      <c r="L28" s="121">
         <f t="shared" si="5"/>
         <v>0.66720500000000005</v>
       </c>
-      <c r="M28" s="139">
+      <c r="M28" s="122">
         <f t="shared" si="6"/>
         <v>1.9851049999999999</v>
       </c>
-      <c r="N28" s="140">
+      <c r="N28" s="123">
         <f t="shared" si="7"/>
         <v>-1.8469600000000002</v>
       </c>
@@ -61388,29 +61389,29 @@
       <c r="D29" s="96">
         <v>-1.86</v>
       </c>
-      <c r="E29" s="151" t="s">
+      <c r="E29" s="144" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="152"/>
-      <c r="G29" s="153"/>
-      <c r="H29" s="110">
+      <c r="F29" s="145"/>
+      <c r="G29" s="146"/>
+      <c r="H29" s="102">
         <v>6.8900000000000003E-2</v>
       </c>
-      <c r="I29" s="111">
+      <c r="I29" s="103">
         <v>8.3500000000000005E-2</v>
       </c>
-      <c r="J29" s="112">
+      <c r="J29" s="104">
         <v>-4.3499999999999997E-2</v>
       </c>
-      <c r="L29" s="141">
+      <c r="L29" s="124">
         <f t="shared" si="5"/>
         <v>-1.5234449999999999</v>
       </c>
-      <c r="M29" s="142">
+      <c r="M29" s="125">
         <f t="shared" si="6"/>
         <v>-1.744175</v>
       </c>
-      <c r="N29" s="143">
+      <c r="N29" s="126">
         <f t="shared" si="7"/>
         <v>-1.8578250000000001</v>
       </c>
@@ -61419,9 +61420,9 @@
       <c r="B30" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="144"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="144"/>
+      <c r="E30" s="147"/>
+      <c r="F30" s="147"/>
+      <c r="G30" s="147"/>
       <c r="H30" t="s">
         <v>49</v>
       </c>
@@ -61431,15 +61432,29 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="H19:J24"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E28:G28"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E26:G26"/>
     <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="H19:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D1CBDF-495C-449C-91A1-AC057764C2B9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>